<commit_message>
Ideal gas handling and flow level additions
</commit_message>
<xml_diff>
--- a/Tests/Cengel_Formatted_Unified.xlsx
+++ b/Tests/Cengel_Formatted_Unified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Belgeler\İşler\Thermobrig\Thermodynamic Property Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE1CA5A-C38B-4AAB-AEAD-0B90BCF87ACF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6622EC4C-BF58-4A22-9E87-BF871928C2B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14235" yWindow="2175" windowWidth="28800" windowHeight="15600" tabRatio="684" activeTab="8" xr2:uid="{7E0FCBEC-8334-4956-96C6-6D7FEAB3F24F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" tabRatio="684" firstSheet="5" activeTab="9" xr2:uid="{7E0FCBEC-8334-4956-96C6-6D7FEAB3F24F}"/>
   </bookViews>
   <sheets>
     <sheet name="SatWater_T" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="SatR134a_P" sheetId="8" r:id="rId7"/>
     <sheet name="SuphR134a" sheetId="9" r:id="rId8"/>
     <sheet name="R134aUnified" sheetId="10" r:id="rId9"/>
-    <sheet name="IAir" sheetId="5" r:id="rId10"/>
+    <sheet name="Air" sheetId="5" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'R134aUnified'!$A$2:$G$444</definedName>
@@ -111,10 +111,10 @@
     <t>mu_r</t>
   </si>
   <si>
-    <t>s^0</t>
+    <t>x</t>
   </si>
   <si>
-    <t>x</t>
+    <t>s0</t>
   </si>
 </sst>
 </file>
@@ -280,7 +280,7 @@
     <tableColumn id="3" xr3:uid="{907EA68A-E67A-4EAB-89CB-AF7A83387DEB}" name="P_r"/>
     <tableColumn id="4" xr3:uid="{A30C02E6-C1E8-4FD8-993B-D06E8FE0EDAC}" name="u"/>
     <tableColumn id="5" xr3:uid="{B5C2015E-06DD-4DAA-BC45-E996D53C55DE}" name="mu_r"/>
-    <tableColumn id="6" xr3:uid="{D3B8AD1D-F451-445C-976D-037647135F75}" name="s^0"/>
+    <tableColumn id="6" xr3:uid="{D3B8AD1D-F451-445C-976D-037647135F75}" name="s0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -641,7 +641,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -662,7 +662,7 @@
         <v>0</v>
       </c>
       <c r="T2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U2" s="5" t="s">
         <v>4</v>
@@ -4050,8 +4050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F916BCB-461F-4634-AF9B-521DDFF433C3}">
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4089,7 +4089,7 @@
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -6587,7 +6587,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -6608,7 +6608,7 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S2" t="s">
         <v>11</v>
@@ -9898,7 +9898,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -22501,7 +22501,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -25126,7 +25126,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -47215,7 +47215,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -47236,7 +47236,7 @@
         <v>0</v>
       </c>
       <c r="T2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U2" s="5" t="s">
         <v>4</v>
@@ -49776,7 +49776,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -49797,7 +49797,7 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S2" t="s">
         <v>11</v>
@@ -51351,7 +51351,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -57405,7 +57405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{651E17BA-A332-4171-9566-87FD2F5487F7}">
   <dimension ref="A1:G444"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A428" workbookViewId="0">
+    <sheetView topLeftCell="A428" workbookViewId="0">
       <selection activeCell="B161" sqref="B161"/>
     </sheetView>
   </sheetViews>
@@ -57439,7 +57439,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Ideal gas processes updates
</commit_message>
<xml_diff>
--- a/Tests/Cengel_Formatted_Unified.xlsx
+++ b/Tests/Cengel_Formatted_Unified.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Belgeler\İşler\Thermobrig\Thermodynamic Property Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\PycharmProjects\Thermobrig\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6622EC4C-BF58-4A22-9E87-BF871928C2B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03E9F96-9AF3-4933-9E8C-9D367BF9D330}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" tabRatio="684" firstSheet="5" activeTab="9" xr2:uid="{7E0FCBEC-8334-4956-96C6-6D7FEAB3F24F}"/>
+    <workbookView xWindow="28680" yWindow="-1275" windowWidth="29040" windowHeight="15990" tabRatio="684" firstSheet="5" activeTab="9" xr2:uid="{7E0FCBEC-8334-4956-96C6-6D7FEAB3F24F}"/>
   </bookViews>
   <sheets>
     <sheet name="SatWater_T" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -102,9 +105,6 @@
     <t>kJ/g</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>P_r</t>
   </si>
   <si>
@@ -116,12 +116,15 @@
   <si>
     <t>s0</t>
   </si>
+  <si>
+    <t>°C</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +137,13 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="162"/>
@@ -641,7 +651,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -662,7 +672,7 @@
         <v>0</v>
       </c>
       <c r="T2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U2" s="5" t="s">
         <v>4</v>
@@ -4050,15 +4060,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F916BCB-461F-4634-AF9B-521DDFF433C3}">
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -4080,21 +4090,21 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>200</v>
+        <v>-73</v>
       </c>
       <c r="B3">
         <v>199.97</v>
@@ -4114,7 +4124,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>210</v>
+        <v>-63</v>
       </c>
       <c r="B4">
         <v>209.97</v>
@@ -4134,7 +4144,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>220</v>
+        <v>-53</v>
       </c>
       <c r="B5">
         <v>219.97</v>
@@ -4154,7 +4164,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>230</v>
+        <v>-43</v>
       </c>
       <c r="B6">
         <v>230.02</v>
@@ -4174,7 +4184,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>240</v>
+        <v>-33</v>
       </c>
       <c r="B7">
         <v>240.02</v>
@@ -4194,7 +4204,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>250</v>
+        <v>-23</v>
       </c>
       <c r="B8">
         <v>250.05</v>
@@ -4214,7 +4224,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>260</v>
+        <v>-13</v>
       </c>
       <c r="B9">
         <v>260.08999999999997</v>
@@ -4234,7 +4244,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>270</v>
+        <v>-3</v>
       </c>
       <c r="B10">
         <v>270.11</v>
@@ -4254,7 +4264,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>280</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>280.13</v>
@@ -4274,7 +4284,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>285</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>285.14</v>
@@ -4294,7 +4304,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>290</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>290.16000000000003</v>
@@ -4314,7 +4324,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>295</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>295.17</v>
@@ -4334,7 +4344,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>298</v>
+        <v>25</v>
       </c>
       <c r="B15">
         <v>298.18</v>
@@ -4354,7 +4364,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>300</v>
+        <v>27</v>
       </c>
       <c r="B16">
         <v>300.19</v>
@@ -4374,7 +4384,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>305</v>
+        <v>32</v>
       </c>
       <c r="B17">
         <v>305.22000000000003</v>
@@ -4394,7 +4404,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>310</v>
+        <v>37</v>
       </c>
       <c r="B18">
         <v>310.24</v>
@@ -4414,7 +4424,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>315</v>
+        <v>42</v>
       </c>
       <c r="B19">
         <v>315.27</v>
@@ -4434,7 +4444,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>320</v>
+        <v>47</v>
       </c>
       <c r="B20">
         <v>320.29000000000002</v>
@@ -4454,7 +4464,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>325</v>
+        <v>52</v>
       </c>
       <c r="B21">
         <v>325.31</v>
@@ -4474,7 +4484,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>330</v>
+        <v>57</v>
       </c>
       <c r="B22">
         <v>330.34</v>
@@ -4494,7 +4504,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>340</v>
+        <v>67</v>
       </c>
       <c r="B23">
         <v>340.42</v>
@@ -4514,7 +4524,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>350</v>
+        <v>77</v>
       </c>
       <c r="B24">
         <v>350.49</v>
@@ -4534,7 +4544,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>360</v>
+        <v>87</v>
       </c>
       <c r="B25">
         <v>360.58</v>
@@ -4554,7 +4564,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>370</v>
+        <v>97</v>
       </c>
       <c r="B26">
         <v>370.67</v>
@@ -4574,7 +4584,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>380</v>
+        <v>107</v>
       </c>
       <c r="B27">
         <v>380.77</v>
@@ -4594,7 +4604,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>390</v>
+        <v>117</v>
       </c>
       <c r="B28">
         <v>390.88</v>
@@ -4614,7 +4624,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>400</v>
+        <v>127</v>
       </c>
       <c r="B29">
         <v>400.98</v>
@@ -4634,7 +4644,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>410</v>
+        <v>137</v>
       </c>
       <c r="B30">
         <v>411.12</v>
@@ -4654,7 +4664,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>420</v>
+        <v>147</v>
       </c>
       <c r="B31">
         <v>421.26</v>
@@ -4674,7 +4684,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>430</v>
+        <v>157</v>
       </c>
       <c r="B32">
         <v>431.43</v>
@@ -4694,7 +4704,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>440</v>
+        <v>167</v>
       </c>
       <c r="B33">
         <v>441.61</v>
@@ -4714,7 +4724,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>450</v>
+        <v>177</v>
       </c>
       <c r="B34">
         <v>451.8</v>
@@ -4734,7 +4744,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>460</v>
+        <v>187</v>
       </c>
       <c r="B35">
         <v>462.02</v>
@@ -4754,7 +4764,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>470</v>
+        <v>197</v>
       </c>
       <c r="B36">
         <v>472.24</v>
@@ -4774,7 +4784,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>480</v>
+        <v>207</v>
       </c>
       <c r="B37">
         <v>482.49</v>
@@ -4794,7 +4804,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>490</v>
+        <v>217</v>
       </c>
       <c r="B38">
         <v>492.74</v>
@@ -4814,7 +4824,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>500</v>
+        <v>227</v>
       </c>
       <c r="B39">
         <v>503.02</v>
@@ -4834,7 +4844,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>510</v>
+        <v>237</v>
       </c>
       <c r="B40">
         <v>513.32000000000005</v>
@@ -4854,7 +4864,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>520</v>
+        <v>247</v>
       </c>
       <c r="B41">
         <v>523.63</v>
@@ -4874,7 +4884,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>530</v>
+        <v>257</v>
       </c>
       <c r="B42">
         <v>533.98</v>
@@ -4894,7 +4904,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>540</v>
+        <v>267</v>
       </c>
       <c r="B43">
         <v>544.35</v>
@@ -4914,7 +4924,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>550</v>
+        <v>277</v>
       </c>
       <c r="B44">
         <v>555.74</v>
@@ -4934,7 +4944,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>560</v>
+        <v>287</v>
       </c>
       <c r="B45">
         <v>565.16999999999996</v>
@@ -4954,7 +4964,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>570</v>
+        <v>297</v>
       </c>
       <c r="B46">
         <v>575.59</v>
@@ -4974,7 +4984,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>580</v>
+        <v>307</v>
       </c>
       <c r="B47">
         <v>586.04</v>
@@ -4994,7 +5004,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>590</v>
+        <v>317</v>
       </c>
       <c r="B48">
         <v>596.52</v>
@@ -5014,7 +5024,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>600</v>
+        <v>327</v>
       </c>
       <c r="B49">
         <v>607.02</v>
@@ -5034,7 +5044,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>610</v>
+        <v>337</v>
       </c>
       <c r="B50">
         <v>617.53</v>
@@ -5054,7 +5064,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>620</v>
+        <v>347</v>
       </c>
       <c r="B51">
         <v>628.07000000000005</v>
@@ -5074,7 +5084,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>630</v>
+        <v>357</v>
       </c>
       <c r="B52">
         <v>638.63</v>
@@ -5094,7 +5104,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>640</v>
+        <v>367</v>
       </c>
       <c r="B53">
         <v>649.22</v>
@@ -5114,7 +5124,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>650</v>
+        <v>377</v>
       </c>
       <c r="B54">
         <v>659.84</v>
@@ -5134,7 +5144,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>660</v>
+        <v>387</v>
       </c>
       <c r="B55">
         <v>670.47</v>
@@ -5154,7 +5164,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>670</v>
+        <v>397</v>
       </c>
       <c r="B56">
         <v>681.14</v>
@@ -5174,7 +5184,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>680</v>
+        <v>407</v>
       </c>
       <c r="B57">
         <v>691.82</v>
@@ -5194,7 +5204,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>690</v>
+        <v>417</v>
       </c>
       <c r="B58">
         <v>702.52</v>
@@ -5214,7 +5224,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>700</v>
+        <v>427</v>
       </c>
       <c r="B59">
         <v>713.27</v>
@@ -5234,7 +5244,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>710</v>
+        <v>437</v>
       </c>
       <c r="B60">
         <v>724.04</v>
@@ -5254,7 +5264,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>720</v>
+        <v>447</v>
       </c>
       <c r="B61">
         <v>734.82</v>
@@ -5274,7 +5284,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>730</v>
+        <v>457</v>
       </c>
       <c r="B62">
         <v>745.62</v>
@@ -5294,7 +5304,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>740</v>
+        <v>467</v>
       </c>
       <c r="B63">
         <v>756.44</v>
@@ -5314,7 +5324,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>750</v>
+        <v>477</v>
       </c>
       <c r="B64">
         <v>767.29</v>
@@ -5334,7 +5344,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>760</v>
+        <v>487</v>
       </c>
       <c r="B65">
         <v>778.18</v>
@@ -5354,7 +5364,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>780</v>
+        <v>507</v>
       </c>
       <c r="B66">
         <v>800.03</v>
@@ -5374,7 +5384,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>800</v>
+        <v>527</v>
       </c>
       <c r="B67">
         <v>821.95</v>
@@ -5394,7 +5404,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>820</v>
+        <v>547</v>
       </c>
       <c r="B68">
         <v>843.98</v>
@@ -5414,7 +5424,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>840</v>
+        <v>567</v>
       </c>
       <c r="B69">
         <v>866.08</v>
@@ -5434,7 +5444,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>860</v>
+        <v>587</v>
       </c>
       <c r="B70">
         <v>888.27</v>
@@ -5454,7 +5464,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>880</v>
+        <v>607</v>
       </c>
       <c r="B71">
         <v>910.56</v>
@@ -5474,7 +5484,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>900</v>
+        <v>627</v>
       </c>
       <c r="B72">
         <v>932.93</v>
@@ -5494,7 +5504,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>920</v>
+        <v>647</v>
       </c>
       <c r="B73">
         <v>955.38</v>
@@ -5514,7 +5524,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>940</v>
+        <v>667</v>
       </c>
       <c r="B74">
         <v>977.92</v>
@@ -5534,7 +5544,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>960</v>
+        <v>687</v>
       </c>
       <c r="B75">
         <v>1000.55</v>
@@ -5554,7 +5564,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>980</v>
+        <v>707</v>
       </c>
       <c r="B76">
         <v>1023.25</v>
@@ -5574,7 +5584,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>1000</v>
+        <v>727</v>
       </c>
       <c r="B77">
         <v>1046.04</v>
@@ -5594,7 +5604,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>1020</v>
+        <v>747</v>
       </c>
       <c r="B78">
         <v>1068.8900000000001</v>
@@ -5614,7 +5624,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>1040</v>
+        <v>767</v>
       </c>
       <c r="B79">
         <v>1091.8499999999999</v>
@@ -5634,7 +5644,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>1060</v>
+        <v>787</v>
       </c>
       <c r="B80">
         <v>1114.8599999999999</v>
@@ -5654,7 +5664,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>1080</v>
+        <v>807</v>
       </c>
       <c r="B81">
         <v>1137.8900000000001</v>
@@ -5674,7 +5684,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>1100</v>
+        <v>827</v>
       </c>
       <c r="B82">
         <v>1161.07</v>
@@ -5694,7 +5704,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>1120</v>
+        <v>847</v>
       </c>
       <c r="B83">
         <v>1184.28</v>
@@ -5714,7 +5724,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>1140</v>
+        <v>867</v>
       </c>
       <c r="B84">
         <v>1207.57</v>
@@ -5734,7 +5744,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>1160</v>
+        <v>887</v>
       </c>
       <c r="B85">
         <v>1230.92</v>
@@ -5754,7 +5764,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>1180</v>
+        <v>907</v>
       </c>
       <c r="B86">
         <v>1254.3399999999999</v>
@@ -5774,7 +5784,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>1200</v>
+        <v>927</v>
       </c>
       <c r="B87">
         <v>1277.79</v>
@@ -5794,7 +5804,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>1220</v>
+        <v>947</v>
       </c>
       <c r="B88">
         <v>1301.31</v>
@@ -5814,7 +5824,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>1240</v>
+        <v>967</v>
       </c>
       <c r="B89">
         <v>1324.93</v>
@@ -5834,7 +5844,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>1260</v>
+        <v>987</v>
       </c>
       <c r="B90">
         <v>1348.55</v>
@@ -5854,7 +5864,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>1280</v>
+        <v>1007</v>
       </c>
       <c r="B91">
         <v>1372.24</v>
@@ -5874,7 +5884,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>1300</v>
+        <v>1027</v>
       </c>
       <c r="B92">
         <v>1395.97</v>
@@ -5894,7 +5904,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>1320</v>
+        <v>1047</v>
       </c>
       <c r="B93">
         <v>1419.76</v>
@@ -5914,7 +5924,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>1340</v>
+        <v>1067</v>
       </c>
       <c r="B94">
         <v>1443.6</v>
@@ -5934,7 +5944,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>1360</v>
+        <v>1087</v>
       </c>
       <c r="B95">
         <v>1467.49</v>
@@ -5954,7 +5964,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>1380</v>
+        <v>1107</v>
       </c>
       <c r="B96">
         <v>1491.44</v>
@@ -5974,7 +5984,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>1400</v>
+        <v>1127</v>
       </c>
       <c r="B97">
         <v>1515.42</v>
@@ -5994,7 +6004,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>1420</v>
+        <v>1147</v>
       </c>
       <c r="B98">
         <v>1539.44</v>
@@ -6014,7 +6024,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>1440</v>
+        <v>1167</v>
       </c>
       <c r="B99">
         <v>1563.51</v>
@@ -6034,7 +6044,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>1460</v>
+        <v>1187</v>
       </c>
       <c r="B100">
         <v>1587.63</v>
@@ -6054,7 +6064,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>1480</v>
+        <v>1207</v>
       </c>
       <c r="B101">
         <v>1611.79</v>
@@ -6074,7 +6084,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>1500</v>
+        <v>1227</v>
       </c>
       <c r="B102">
         <v>1635.97</v>
@@ -6094,7 +6104,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>1520</v>
+        <v>1247</v>
       </c>
       <c r="B103">
         <v>1660.23</v>
@@ -6114,7 +6124,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>1540</v>
+        <v>1267</v>
       </c>
       <c r="B104">
         <v>1684.51</v>
@@ -6134,7 +6144,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>1560</v>
+        <v>1287</v>
       </c>
       <c r="B105">
         <v>1708.82</v>
@@ -6154,7 +6164,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>1580</v>
+        <v>1307</v>
       </c>
       <c r="B106">
         <v>1733.17</v>
@@ -6174,7 +6184,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>1600</v>
+        <v>1327</v>
       </c>
       <c r="B107">
         <v>1757.57</v>
@@ -6194,7 +6204,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>1620</v>
+        <v>1347</v>
       </c>
       <c r="B108">
         <v>1782</v>
@@ -6214,7 +6224,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>1640</v>
+        <v>1367</v>
       </c>
       <c r="B109">
         <v>1806.46</v>
@@ -6234,7 +6244,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>1660</v>
+        <v>1387</v>
       </c>
       <c r="B110">
         <v>1830.96</v>
@@ -6254,7 +6264,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>1680</v>
+        <v>1407</v>
       </c>
       <c r="B111">
         <v>1855.5</v>
@@ -6274,7 +6284,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>1700</v>
+        <v>1427</v>
       </c>
       <c r="B112">
         <v>1880.1</v>
@@ -6294,7 +6304,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>1750</v>
+        <v>1477</v>
       </c>
       <c r="B113">
         <v>1941.6</v>
@@ -6314,7 +6324,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>1800</v>
+        <v>1527</v>
       </c>
       <c r="B114">
         <v>2003.3</v>
@@ -6334,7 +6344,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>1850</v>
+        <v>1577</v>
       </c>
       <c r="B115">
         <v>2065.3000000000002</v>
@@ -6354,7 +6364,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>1900</v>
+        <v>1627</v>
       </c>
       <c r="B116">
         <v>2127.4</v>
@@ -6374,7 +6384,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>1950</v>
+        <v>1677</v>
       </c>
       <c r="B117">
         <v>2189.6999999999998</v>
@@ -6394,7 +6404,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>2000</v>
+        <v>1727</v>
       </c>
       <c r="B118">
         <v>2252.1</v>
@@ -6414,7 +6424,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>2050</v>
+        <v>1777</v>
       </c>
       <c r="B119">
         <v>2314.6</v>
@@ -6434,7 +6444,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>2100</v>
+        <v>1827</v>
       </c>
       <c r="B120">
         <v>2377.6999999999998</v>
@@ -6454,7 +6464,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>2150</v>
+        <v>1877</v>
       </c>
       <c r="B121">
         <v>2440.3000000000002</v>
@@ -6474,7 +6484,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>2200</v>
+        <v>1927</v>
       </c>
       <c r="B122">
         <v>2503.1999999999998</v>
@@ -6494,7 +6504,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>2250</v>
+        <v>1977</v>
       </c>
       <c r="B123">
         <v>2566.4</v>
@@ -6513,6 +6523,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A3:A123">
     <cfRule type="colorScale" priority="1">
       <colorScale>
@@ -6587,7 +6598,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -6608,7 +6619,7 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S2" t="s">
         <v>11</v>
@@ -9898,7 +9909,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -22501,7 +22512,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -25126,7 +25137,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -47215,7 +47226,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -47236,7 +47247,7 @@
         <v>0</v>
       </c>
       <c r="T2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U2" s="5" t="s">
         <v>4</v>
@@ -49776,7 +49787,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -49797,7 +49808,7 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S2" t="s">
         <v>11</v>
@@ -51351,7 +51362,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -57439,7 +57450,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>

</xml_diff>